<commit_message>
Update São Tomé e Príncipe export direct reporting
</commit_message>
<xml_diff>
--- a/reports/Sao Tome and Principe_1.1_trade_balance_2003-2023.xlsx
+++ b/reports/Sao Tome and Principe_1.1_trade_balance_2003-2023.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrc/develop/cipf-comtrade/reports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB299C7-B0E5-D144-B9F8-8A9B9D13ED55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="4860" yWindow="500" windowWidth="26020" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -115,8 +121,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +136,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -165,27 +182,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -223,7 +255,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -257,6 +289,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -291,9 +324,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,14 +500,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.83203125" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -501,746 +544,746 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>40833591</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>57970761.169</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>6628901</v>
       </c>
-      <c r="E2">
-        <v>13503048.208</v>
-      </c>
-      <c r="F2">
+      <c r="E2" s="2">
+        <v>13503048.208000001</v>
+      </c>
+      <c r="F2" s="2">
         <v>-34204690</v>
       </c>
-      <c r="G2">
-        <v>-27330542.792</v>
-      </c>
-      <c r="H2">
+      <c r="G2" s="2">
+        <v>-27330542.791999999</v>
+      </c>
+      <c r="H2" s="2">
         <v>47462492</v>
       </c>
-      <c r="I2">
-        <v>54336639.208</v>
-      </c>
-      <c r="J2">
+      <c r="I2" s="2">
+        <v>54336639.207999997</v>
+      </c>
+      <c r="J2" s="4">
         <v>0.7043825227852254</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="4">
         <v>0.4909188575711852</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>41433788</v>
       </c>
-      <c r="C3">
-        <v>60386982.132</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="2">
+        <v>60386982.131999999</v>
+      </c>
+      <c r="D3" s="2">
         <v>3553080</v>
       </c>
-      <c r="E3">
-        <v>12927308.391</v>
-      </c>
-      <c r="F3">
+      <c r="E3" s="2">
+        <v>12927308.391000001</v>
+      </c>
+      <c r="F3" s="2">
         <v>-37880708</v>
       </c>
-      <c r="G3">
-        <v>-28506479.609</v>
-      </c>
-      <c r="H3">
+      <c r="G3" s="2">
+        <v>-28506479.609000001</v>
+      </c>
+      <c r="H3" s="2">
         <v>44986868</v>
       </c>
-      <c r="I3">
-        <v>54361096.391</v>
-      </c>
-      <c r="J3">
-        <v>0.6861377491829251</v>
-      </c>
-      <c r="K3">
-        <v>0.2748507185357825</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="I3" s="2">
+        <v>54361096.391000003</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.68613774918292514</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.27485071853578252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>49860404</v>
       </c>
-      <c r="C4">
-        <v>60036165.701</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="2">
+        <v>60036165.700999998</v>
+      </c>
+      <c r="D4" s="2">
         <v>3416365</v>
       </c>
-      <c r="E4">
-        <v>12096305.95</v>
-      </c>
-      <c r="F4">
+      <c r="E4" s="2">
+        <v>12096305.949999999</v>
+      </c>
+      <c r="F4" s="2">
         <v>-46444039</v>
       </c>
-      <c r="G4">
-        <v>-37764098.05</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="2">
+        <v>-37764098.049999997</v>
+      </c>
+      <c r="H4" s="2">
         <v>53276769</v>
       </c>
-      <c r="I4">
-        <v>61956709.95</v>
-      </c>
-      <c r="J4">
-        <v>0.8305061360567452</v>
-      </c>
-      <c r="K4">
-        <v>0.2824304390217577</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="I4" s="2">
+        <v>61956709.950000003</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.83050613605674517</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.28243043902175768</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>71135517</v>
       </c>
-      <c r="C5">
-        <v>72451314.626</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="2">
+        <v>72451314.626000002</v>
+      </c>
+      <c r="D5" s="2">
         <v>3873963</v>
       </c>
-      <c r="E5">
-        <v>21248305.806</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="2">
+        <v>21248305.806000002</v>
+      </c>
+      <c r="F5" s="2">
         <v>-67261554</v>
       </c>
-      <c r="G5">
-        <v>-49887211.194</v>
-      </c>
-      <c r="H5">
+      <c r="G5" s="2">
+        <v>-49887211.193999998</v>
+      </c>
+      <c r="H5" s="2">
         <v>75009480</v>
       </c>
-      <c r="I5">
-        <v>92383822.80599999</v>
-      </c>
-      <c r="J5">
-        <v>0.9818388716230718</v>
-      </c>
-      <c r="K5">
-        <v>0.1823186768568668</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="I5" s="2">
+        <v>92383822.805999994</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.98183887162307182</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0.18231867685686681</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>79418250</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>107557254.418</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>6729006</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>11952798.362</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>-72689244</v>
       </c>
-      <c r="G6">
-        <v>-67465451.638</v>
-      </c>
-      <c r="H6">
+      <c r="G6" s="2">
+        <v>-67465451.637999997</v>
+      </c>
+      <c r="H6" s="2">
         <v>86147256</v>
       </c>
-      <c r="I6">
-        <v>91371048.362</v>
-      </c>
-      <c r="J6">
-        <v>0.7383811573634697</v>
-      </c>
-      <c r="K6">
-        <v>0.562964905472903</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="I6" s="2">
+        <v>91371048.362000003</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.73838115736346965</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0.56296490547290301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>114045081</v>
       </c>
-      <c r="C7">
-        <v>97132777.37100001</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="2">
+        <v>97132777.371000007</v>
+      </c>
+      <c r="D7" s="2">
         <v>10631930</v>
       </c>
-      <c r="E7">
-        <v>9702483.521</v>
-      </c>
-      <c r="F7">
+      <c r="E7" s="2">
+        <v>9702483.5209999997</v>
+      </c>
+      <c r="F7" s="2">
         <v>-103413151</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>-104342597.479</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>124677011</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <v>123747564.521</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="4">
         <v>1.174115309854707</v>
       </c>
-      <c r="K7">
-        <v>1.095794698026367</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="K7" s="4">
+        <v>1.0957946980263671</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>103283149</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>128134929.814</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>8116665</v>
       </c>
-      <c r="E8">
-        <v>18001730.197</v>
-      </c>
-      <c r="F8">
+      <c r="E8" s="2">
+        <v>18001730.197000001</v>
+      </c>
+      <c r="F8" s="2">
         <v>-95166484</v>
       </c>
-      <c r="G8">
-        <v>-85281418.803</v>
-      </c>
-      <c r="H8">
+      <c r="G8" s="2">
+        <v>-85281418.803000003</v>
+      </c>
+      <c r="H8" s="2">
         <v>111399814</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <v>121284879.197</v>
       </c>
-      <c r="J8">
-        <v>0.8060499127749574</v>
-      </c>
-      <c r="K8">
-        <v>0.4508824935812363</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="J8" s="4">
+        <v>0.80604991277495741</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.45088249358123628</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>112152144</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>148107791.014</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>6381277</v>
       </c>
-      <c r="E9">
-        <v>18386131.129</v>
-      </c>
-      <c r="F9">
+      <c r="E9" s="2">
+        <v>18386131.129000001</v>
+      </c>
+      <c r="F9" s="2">
         <v>-105770867</v>
       </c>
-      <c r="G9">
-        <v>-93766012.87099999</v>
-      </c>
-      <c r="H9">
+      <c r="G9" s="2">
+        <v>-93766012.870999992</v>
+      </c>
+      <c r="H9" s="2">
         <v>118533421</v>
       </c>
-      <c r="I9">
-        <v>130538275.129</v>
-      </c>
-      <c r="J9">
-        <v>0.7572332504061096</v>
-      </c>
-      <c r="K9">
-        <v>0.3470701342891526</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="I9" s="2">
+        <v>130538275.12899999</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.75723325040610956</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.34707013428915262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>133712481</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>165008512.567</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>11041542</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>16451985.044</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>-122670939</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>-117260495.956</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>144754023</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="2">
         <v>150164466.044</v>
       </c>
-      <c r="J10">
-        <v>0.8103368663826203</v>
-      </c>
-      <c r="K10">
-        <v>0.6711373715980142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="J10" s="4">
+        <v>0.81033686638262026</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0.67113737159801423</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>141253970</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>130133702.28</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>6047150</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>14234004.338</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>-135206820</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>-127019965.662</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>147301120</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>155487974.338</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="4">
         <v>1.085452634676245</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="4">
         <v>0.4248382855874327</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>152093663</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>135278948.63</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>6938258</v>
       </c>
-      <c r="E12">
-        <v>10288119.81</v>
-      </c>
-      <c r="F12">
+      <c r="E12" s="2">
+        <v>10288119.810000001</v>
+      </c>
+      <c r="F12" s="2">
         <v>-145155405</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>-141805543.19</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>159031921</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="2">
         <v>162381782.81</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="4">
         <v>1.124296607419605</v>
       </c>
-      <c r="K12">
-        <v>0.6743951400387123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="K12" s="4">
+        <v>0.67439514003871226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>169715687</v>
       </c>
-      <c r="C13">
-        <v>154273138.712</v>
-      </c>
-      <c r="D13">
+      <c r="C13" s="2">
+        <v>154273138.71200001</v>
+      </c>
+      <c r="D13" s="2">
         <v>10497358</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>16332217.263</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>-159218329</v>
       </c>
-      <c r="G13">
-        <v>-153383469.737</v>
-      </c>
-      <c r="H13">
+      <c r="G13" s="2">
+        <v>-153383469.73699999</v>
+      </c>
+      <c r="H13" s="2">
         <v>180213045</v>
       </c>
-      <c r="I13">
-        <v>186047904.263</v>
-      </c>
-      <c r="J13">
+      <c r="I13" s="2">
+        <v>186047904.26300001</v>
+      </c>
+      <c r="J13" s="4">
         <v>1.10009874963929</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="4">
         <v>0.642739306669729</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>141847245</v>
       </c>
-      <c r="C14">
-        <v>134413702.302</v>
-      </c>
-      <c r="D14">
+      <c r="C14" s="2">
+        <v>134413702.30199999</v>
+      </c>
+      <c r="D14" s="2">
         <v>9223182</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>14570628.521</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>-132624063</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>-127276616.479</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <v>151070427</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <v>156417873.521</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="4">
         <v>1.055303459176345</v>
       </c>
-      <c r="K14">
-        <v>0.6329982256226653</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="K14" s="4">
+        <v>0.63299822562266528</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>139352022</v>
       </c>
-      <c r="C15">
-        <v>139051314.48</v>
-      </c>
-      <c r="D15">
+      <c r="C15" s="2">
+        <v>139051314.47999999</v>
+      </c>
+      <c r="D15" s="2">
         <v>10473934</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>22420018.23</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>-128878088</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>-116932003.77</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="2">
         <v>149825956</v>
       </c>
-      <c r="I15">
-        <v>161772040.23</v>
-      </c>
-      <c r="J15">
+      <c r="I15" s="2">
+        <v>161772040.22999999</v>
+      </c>
+      <c r="J15" s="4">
         <v>1.002162565101413</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="4">
         <v>0.4671688440460291</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16">
-        <v>147049579.311</v>
-      </c>
-      <c r="C16">
-        <v>135633758.561</v>
-      </c>
-      <c r="D16">
-        <v>10562590.924</v>
-      </c>
-      <c r="E16">
+      <c r="B16" s="2">
+        <v>147049579.31099999</v>
+      </c>
+      <c r="C16" s="2">
+        <v>135633758.56099999</v>
+      </c>
+      <c r="D16" s="2">
+        <v>10562590.924000001</v>
+      </c>
+      <c r="E16" s="2">
         <v>14354580.753</v>
       </c>
-      <c r="F16">
-        <v>-136486988.387</v>
-      </c>
-      <c r="G16">
+      <c r="F16" s="2">
+        <v>-136486988.38699999</v>
+      </c>
+      <c r="G16" s="2">
         <v>-132694998.558</v>
       </c>
-      <c r="H16">
-        <v>157612170.235</v>
-      </c>
-      <c r="I16">
-        <v>161404160.064</v>
-      </c>
-      <c r="J16">
-        <v>1.084166514819877</v>
-      </c>
-      <c r="K16">
-        <v>0.7358341637245308</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="H16" s="2">
+        <v>157612170.23500001</v>
+      </c>
+      <c r="I16" s="2">
+        <v>161404160.06400001</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1.0841665148198769</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0.73583416372453081</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17">
-        <v>148305957.032</v>
-      </c>
-      <c r="C17">
-        <v>143037169.881</v>
-      </c>
-      <c r="D17">
+      <c r="B17" s="2">
+        <v>148305957.03200001</v>
+      </c>
+      <c r="C17" s="2">
+        <v>143037169.88100001</v>
+      </c>
+      <c r="D17" s="2">
         <v>12087302.455</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>17100216.309</v>
       </c>
-      <c r="F17">
-        <v>-136218654.577</v>
-      </c>
-      <c r="G17">
+      <c r="F17" s="2">
+        <v>-136218654.57699999</v>
+      </c>
+      <c r="G17" s="2">
         <v>-131205740.723</v>
       </c>
-      <c r="H17">
-        <v>160393259.487</v>
-      </c>
-      <c r="I17">
-        <v>165406173.341</v>
-      </c>
-      <c r="J17">
+      <c r="H17" s="2">
+        <v>160393259.48699999</v>
+      </c>
+      <c r="I17" s="2">
+        <v>165406173.34099999</v>
+      </c>
+      <c r="J17" s="4">
         <v>1.036835090874515</v>
       </c>
-      <c r="K17">
-        <v>0.7068508512748077</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="K17" s="4">
+        <v>0.70685085127480773</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>147666945.396</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>148733419.074</v>
       </c>
-      <c r="D18">
-        <v>9858888.949999999</v>
-      </c>
-      <c r="E18">
-        <v>23800547.964</v>
-      </c>
-      <c r="F18">
-        <v>-137808056.446</v>
-      </c>
-      <c r="G18">
+      <c r="D18" s="2">
+        <v>9858888.9499999993</v>
+      </c>
+      <c r="E18" s="2">
+        <v>23800547.964000002</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-137808056.44600001</v>
+      </c>
+      <c r="G18" s="2">
         <v>-123866397.432</v>
       </c>
-      <c r="H18">
-        <v>157525834.346</v>
-      </c>
-      <c r="I18">
-        <v>171467493.36</v>
-      </c>
-      <c r="J18">
-        <v>0.9928296297856947</v>
-      </c>
-      <c r="K18">
-        <v>0.4142294944180387</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="H18" s="2">
+        <v>157525834.34599999</v>
+      </c>
+      <c r="I18" s="2">
+        <v>171467493.36000001</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.99282962978569467</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0.41422949441803869</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B19">
-        <v>138041161.357</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="2">
+        <v>138041161.35699999</v>
+      </c>
+      <c r="C19" s="2">
         <v>118517373.594</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>12439557.111</v>
       </c>
-      <c r="E19">
-        <v>26293343.023</v>
-      </c>
-      <c r="F19">
-        <v>-125601604.246</v>
-      </c>
-      <c r="G19">
-        <v>-111747818.334</v>
-      </c>
-      <c r="H19">
-        <v>150480718.468</v>
-      </c>
-      <c r="I19">
+      <c r="E19" s="2">
+        <v>26293343.022999998</v>
+      </c>
+      <c r="F19" s="2">
+        <v>-125601604.24600001</v>
+      </c>
+      <c r="G19" s="2">
+        <v>-111747818.33400001</v>
+      </c>
+      <c r="H19" s="2">
+        <v>150480718.46799999</v>
+      </c>
+      <c r="I19" s="2">
         <v>164334504.38</v>
       </c>
-      <c r="J19">
-        <v>1.164733550625935</v>
-      </c>
-      <c r="K19">
-        <v>0.4731067137457016</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="J19" s="4">
+        <v>1.1647335506259351</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0.47310671374570162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B20">
-        <v>166275006.874</v>
-      </c>
-      <c r="C20">
+      <c r="B20" s="2">
+        <v>166275006.87400001</v>
+      </c>
+      <c r="C20" s="2">
         <v>132773235.888</v>
       </c>
-      <c r="D20">
-        <v>19174845.703</v>
-      </c>
-      <c r="E20">
-        <v>29185861.306</v>
-      </c>
-      <c r="F20">
+      <c r="D20" s="2">
+        <v>19174845.703000002</v>
+      </c>
+      <c r="E20" s="2">
+        <v>29185861.306000002</v>
+      </c>
+      <c r="F20" s="2">
         <v>-147100161.171</v>
       </c>
-      <c r="G20">
-        <v>-137089145.568</v>
-      </c>
-      <c r="H20">
-        <v>185449852.577</v>
-      </c>
-      <c r="I20">
-        <v>195460868.18</v>
-      </c>
-      <c r="J20">
+      <c r="G20" s="2">
+        <v>-137089145.56799999</v>
+      </c>
+      <c r="H20" s="2">
+        <v>185449852.57699999</v>
+      </c>
+      <c r="I20" s="2">
+        <v>195460868.18000001</v>
+      </c>
+      <c r="J20" s="4">
         <v>1.252323224345155</v>
       </c>
-      <c r="K20">
-        <v>0.6569909142636149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="K20" s="4">
+        <v>0.65699091426361489</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B21">
-        <v>196299315.483</v>
-      </c>
-      <c r="C21">
-        <v>169470201.798</v>
-      </c>
-      <c r="D21">
-        <v>22588961.006</v>
-      </c>
-      <c r="E21">
-        <v>22554933.31</v>
-      </c>
-      <c r="F21">
+      <c r="B21" s="2">
+        <v>196299315.48300001</v>
+      </c>
+      <c r="C21" s="2">
+        <v>169470201.79800001</v>
+      </c>
+      <c r="D21" s="2">
+        <v>22588961.006000001</v>
+      </c>
+      <c r="E21" s="2">
+        <v>22554933.309999999</v>
+      </c>
+      <c r="F21" s="2">
         <v>-173710354.477</v>
       </c>
-      <c r="G21">
-        <v>-173744382.173</v>
-      </c>
-      <c r="H21">
-        <v>218888276.489</v>
-      </c>
-      <c r="I21">
-        <v>218854248.793</v>
-      </c>
-      <c r="J21">
-        <v>1.158311687838662</v>
-      </c>
-      <c r="K21">
-        <v>1.001508658683771</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="G21" s="2">
+        <v>-173744382.17300001</v>
+      </c>
+      <c r="H21" s="2">
+        <v>218888276.48899999</v>
+      </c>
+      <c r="I21" s="2">
+        <v>218854248.79300001</v>
+      </c>
+      <c r="J21" s="4">
+        <v>1.1583116878386619</v>
+      </c>
+      <c r="K21" s="4">
+        <v>1.0015086586837709</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B22">
-        <v>183563238.117</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="2">
+        <v>183563238.11700001</v>
+      </c>
+      <c r="C22" s="2">
         <v>100315818.912</v>
       </c>
-      <c r="D22">
-        <v>16554568.871</v>
-      </c>
-      <c r="E22">
-        <v>53878001.064</v>
-      </c>
-      <c r="F22">
-        <v>-167008669.246</v>
-      </c>
-      <c r="G22">
+      <c r="D22" s="2">
+        <v>16554568.870999999</v>
+      </c>
+      <c r="E22" s="2">
+        <v>53878001.064000003</v>
+      </c>
+      <c r="F22" s="2">
+        <v>-167008669.24599999</v>
+      </c>
+      <c r="G22" s="2">
         <v>-129685237.053</v>
       </c>
-      <c r="H22">
-        <v>200117806.988</v>
-      </c>
-      <c r="I22">
-        <v>237441239.181</v>
-      </c>
-      <c r="J22">
-        <v>1.829853358202928</v>
-      </c>
-      <c r="K22">
-        <v>0.3072602647476722</v>
+      <c r="H22" s="2">
+        <v>200117806.98800001</v>
+      </c>
+      <c r="I22" s="2">
+        <v>237441239.18099999</v>
+      </c>
+      <c r="J22" s="4">
+        <v>1.8298533582029279</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0.30726026474767221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>